<commit_message>
Add daisy chain connection interface.
</commit_message>
<xml_diff>
--- a/LTC6811_ESP32_BOM.xlsx
+++ b/LTC6811_ESP32_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\teTra\BMS\LTC6811_ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752A0DE6-71D7-4A32-AD5C-96356D173542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52406AF6-B56B-4FE7-B5B9-90799248BB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="-13860" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTC6811_ESP32" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="502">
   <si>
     <t>LTC6811_ESP32_BOM</t>
   </si>
@@ -319,9 +319,6 @@
     <t>0603B105K250XD</t>
   </si>
   <si>
-    <t>C53</t>
-  </si>
-  <si>
     <t>100pF 100V</t>
   </si>
   <si>
@@ -1208,9 +1205,6 @@
   </si>
   <si>
     <t>760390014</t>
-  </si>
-  <si>
-    <t>TR2, TR3</t>
   </si>
   <si>
     <t>HM2108NL</t>
@@ -1495,6 +1489,62 @@
   </si>
   <si>
     <t>Resistor_SMD:R_2010_5025Metric</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>J15</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENNOID:Pin_1x02-XL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://tools.molex.com/pdm_docs/sd/705430001_sd.pdf</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connector Header Through Hole 2 position 0.100" (2.54mm)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.digikey.jp/en/products/detail/molex/0705430001/114915?s=N4IgTCBcDaIOwAYCsAWAzAWgdgjCAugL5A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>TR3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>HM2102NL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer_SMD:HM2102NL_PUL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://productfinder.pulseelectronics.com/api/open/part-attachments/datasheet/HM2102NL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>150µH Pulse Transformer 1:1 Surface Mount</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.digikey.jp/en/products/detail/pulse-electronics/HM2102NL/7914608</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C22,C53</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1502,7 +1552,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1556,6 +1606,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1582,7 +1640,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1604,12 +1662,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1618,6 +1670,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2108,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2119,7 +2180,7 @@
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="24.125" style="2" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="21.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.75" style="2" customWidth="1"/>
     <col min="5" max="5" width="32.25" style="2" customWidth="1"/>
     <col min="6" max="6" width="41.625" style="2" customWidth="1"/>
     <col min="7" max="7" width="37.625" style="2" customWidth="1"/>
@@ -2128,28 +2189,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
@@ -2586,33 +2647,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" s="8" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H18" t="s">
-        <v>104</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
+      <c r="I18" s="8">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
@@ -2620,25 +2681,25 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" t="s">
         <v>105</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" t="s">
         <v>110</v>
-      </c>
-      <c r="H19" t="s">
-        <v>111</v>
       </c>
       <c r="I19">
         <v>4</v>
@@ -2649,25 +2710,25 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
         <v>112</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" t="s">
         <v>117</v>
-      </c>
-      <c r="H20" t="s">
-        <v>118</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -2678,25 +2739,25 @@
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
         <v>119</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>124</v>
-      </c>
       <c r="H21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -2707,25 +2768,25 @@
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" t="s">
         <v>125</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" t="s">
         <v>130</v>
-      </c>
-      <c r="H22" t="s">
-        <v>131</v>
       </c>
       <c r="I22">
         <v>2</v>
@@ -2736,25 +2797,25 @@
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" t="s">
         <v>132</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" t="s">
         <v>136</v>
-      </c>
-      <c r="H23" t="s">
-        <v>137</v>
       </c>
       <c r="I23">
         <v>2</v>
@@ -2765,25 +2826,25 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" t="s">
         <v>138</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" t="s">
         <v>143</v>
-      </c>
-      <c r="H24" t="s">
-        <v>144</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -2794,25 +2855,25 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" t="s">
         <v>145</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" t="s">
         <v>150</v>
-      </c>
-      <c r="H25" t="s">
-        <v>151</v>
       </c>
       <c r="I25">
         <v>12</v>
@@ -2823,25 +2884,25 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" t="s">
         <v>152</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="H26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I26">
         <v>14</v>
@@ -2852,25 +2913,25 @@
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" t="s">
         <v>158</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="H27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -2881,25 +2942,25 @@
         <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" t="s">
         <v>164</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="H28" t="s">
         <v>169</v>
-      </c>
-      <c r="H28" t="s">
-        <v>170</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -2910,25 +2971,25 @@
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" t="s">
         <v>171</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" t="s">
         <v>176</v>
-      </c>
-      <c r="H29" t="s">
-        <v>177</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -2939,25 +3000,25 @@
         <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" t="s">
         <v>178</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" t="s">
         <v>183</v>
-      </c>
-      <c r="H30" t="s">
-        <v>184</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -2968,25 +3029,25 @@
         <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" t="s">
         <v>185</v>
       </c>
-      <c r="C31" t="s">
-        <v>186</v>
-      </c>
       <c r="D31" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" t="s">
         <v>176</v>
-      </c>
-      <c r="H31" t="s">
-        <v>177</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2997,25 +3058,25 @@
         <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" t="s">
         <v>187</v>
       </c>
-      <c r="C32" t="s">
-        <v>188</v>
-      </c>
       <c r="D32" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="H32" t="s">
         <v>176</v>
-      </c>
-      <c r="H32" t="s">
-        <v>177</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -3026,16 +3087,16 @@
         <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C33" t="s">
         <v>189</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -3046,16 +3107,16 @@
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C34" t="s">
         <v>193</v>
       </c>
-      <c r="C34" t="s">
-        <v>194</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -3066,19 +3127,19 @@
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" t="s">
         <v>195</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H35" t="s">
         <v>197</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="H35" t="s">
-        <v>198</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -3089,25 +3150,25 @@
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" t="s">
         <v>199</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="H36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I36">
         <v>2</v>
@@ -3118,25 +3179,25 @@
         <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" t="s">
         <v>205</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="H37" t="s">
         <v>210</v>
-      </c>
-      <c r="H37" t="s">
-        <v>211</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -3147,13 +3208,13 @@
         <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C38" t="s">
         <v>212</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -3164,25 +3225,25 @@
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C39" t="s">
         <v>215</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" s="4" t="s">
+      <c r="F39" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>219</v>
-      </c>
       <c r="H39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -3193,25 +3254,25 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C40" t="s">
         <v>220</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="F40" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="H40" t="s">
         <v>225</v>
-      </c>
-      <c r="H40" t="s">
-        <v>226</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -3222,25 +3283,25 @@
         <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C41" t="s">
         <v>227</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="H41" t="s">
         <v>231</v>
-      </c>
-      <c r="H41" t="s">
-        <v>232</v>
       </c>
       <c r="I41">
         <v>12</v>
@@ -3251,25 +3312,25 @@
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C42" t="s">
         <v>233</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="H42" t="s">
         <v>237</v>
-      </c>
-      <c r="H42" t="s">
-        <v>238</v>
       </c>
       <c r="I42">
         <v>3</v>
@@ -3280,25 +3341,25 @@
         <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E43" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="H43" t="s">
         <v>242</v>
-      </c>
-      <c r="H43" t="s">
-        <v>243</v>
       </c>
       <c r="I43">
         <v>4</v>
@@ -3309,25 +3370,25 @@
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C44" t="s">
         <v>244</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="G44" s="4" t="s">
+      <c r="H44" t="s">
         <v>247</v>
-      </c>
-      <c r="H44" t="s">
-        <v>248</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -3338,25 +3399,25 @@
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C45" t="s">
         <v>249</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G45" s="4" t="s">
+      <c r="H45" t="s">
         <v>252</v>
-      </c>
-      <c r="H45" t="s">
-        <v>253</v>
       </c>
       <c r="I45">
         <v>5</v>
@@ -3367,25 +3428,25 @@
         <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="D46" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="F46" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="H46" t="s">
         <v>259</v>
-      </c>
-      <c r="H46" t="s">
-        <v>260</v>
       </c>
       <c r="I46">
         <v>4</v>
@@ -3396,25 +3457,25 @@
         <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C47" t="s">
         <v>261</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="F47" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="H47" t="s">
         <v>266</v>
-      </c>
-      <c r="H47" t="s">
-        <v>267</v>
       </c>
       <c r="I47">
         <v>1</v>
@@ -3425,25 +3486,25 @@
         <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C48" t="s">
         <v>268</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="H48" t="s">
         <v>271</v>
-      </c>
-      <c r="H48" t="s">
-        <v>272</v>
       </c>
       <c r="I48">
         <v>1</v>
@@ -3454,56 +3515,56 @@
         <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C49" t="s">
+        <v>272</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E49" s="4" t="s">
+      <c r="F49" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="H49" t="s">
         <v>276</v>
-      </c>
-      <c r="H49" t="s">
-        <v>277</v>
       </c>
       <c r="I49">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="10" customFormat="1" ht="54" x14ac:dyDescent="0.15">
-      <c r="A50" s="8">
+    <row r="50" spans="1:9" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+      <c r="A50" s="1">
         <v>47</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="E50" s="11" t="s">
+      <c r="G50" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="H50" s="8" t="s">
         <v>481</v>
       </c>
-      <c r="G50" s="11" t="s">
-        <v>482</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="I50" s="10">
+      <c r="I50" s="8">
         <v>1</v>
       </c>
     </row>
@@ -3512,25 +3573,25 @@
         <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C51" t="s">
         <v>278</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="H51" t="s">
         <v>281</v>
-      </c>
-      <c r="H51" t="s">
-        <v>282</v>
       </c>
       <c r="I51">
         <v>1</v>
@@ -3541,25 +3602,25 @@
         <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C52" t="s">
         <v>283</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="H52" t="s">
         <v>286</v>
-      </c>
-      <c r="H52" t="s">
-        <v>287</v>
       </c>
       <c r="I52">
         <v>19</v>
@@ -3570,25 +3631,25 @@
         <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C53" t="s">
         <v>288</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="H53" t="s">
         <v>291</v>
-      </c>
-      <c r="H53" t="s">
-        <v>292</v>
       </c>
       <c r="I53">
         <v>2</v>
@@ -3599,25 +3660,25 @@
         <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C54" t="s">
         <v>293</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="H54" t="s">
         <v>296</v>
-      </c>
-      <c r="H54" t="s">
-        <v>297</v>
       </c>
       <c r="I54">
         <v>14</v>
@@ -3628,25 +3689,25 @@
         <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C55" t="s">
         <v>298</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="H55" t="s">
         <v>301</v>
-      </c>
-      <c r="H55" t="s">
-        <v>302</v>
       </c>
       <c r="I55">
         <v>2</v>
@@ -3657,25 +3718,25 @@
         <v>53</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C56" t="s">
         <v>303</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E56" s="4" t="s">
+      <c r="F56" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="G56" s="4" t="s">
+      <c r="H56" t="s">
         <v>307</v>
-      </c>
-      <c r="H56" t="s">
-        <v>308</v>
       </c>
       <c r="I56">
         <v>1</v>
@@ -3686,25 +3747,25 @@
         <v>54</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C57" t="s">
         <v>309</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="G57" s="4" t="s">
+      <c r="H57" t="s">
         <v>312</v>
-      </c>
-      <c r="H57" t="s">
-        <v>313</v>
       </c>
       <c r="I57">
         <v>1</v>
@@ -3715,25 +3776,25 @@
         <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C58" t="s">
         <v>314</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="H58" t="s">
         <v>317</v>
-      </c>
-      <c r="H58" t="s">
-        <v>318</v>
       </c>
       <c r="I58">
         <v>1</v>
@@ -3744,25 +3805,25 @@
         <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C59" t="s">
         <v>319</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F59" s="2" t="s">
+      <c r="G59" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="H59" t="s">
         <v>322</v>
-      </c>
-      <c r="H59" t="s">
-        <v>323</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -3773,25 +3834,25 @@
         <v>57</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C60" t="s">
         <v>324</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F60" s="2" t="s">
+      <c r="G60" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="H60" t="s">
         <v>327</v>
-      </c>
-      <c r="H60" t="s">
-        <v>328</v>
       </c>
       <c r="I60">
         <v>1</v>
@@ -3802,25 +3863,25 @@
         <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C61" t="s">
         <v>329</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="G61" s="4" t="s">
+      <c r="H61" t="s">
         <v>332</v>
-      </c>
-      <c r="H61" t="s">
-        <v>333</v>
       </c>
       <c r="I61">
         <v>4</v>
@@ -3831,25 +3892,25 @@
         <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C62" t="s">
         <v>334</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F62" s="2" t="s">
+      <c r="G62" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="H62" t="s">
         <v>337</v>
-      </c>
-      <c r="H62" t="s">
-        <v>338</v>
       </c>
       <c r="I62">
         <v>2</v>
@@ -3860,25 +3921,25 @@
         <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="D63" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="H63" t="s">
         <v>342</v>
-      </c>
-      <c r="H63" t="s">
-        <v>343</v>
       </c>
       <c r="I63">
         <v>2</v>
@@ -3889,25 +3950,25 @@
         <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C64" t="s">
         <v>344</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F64" s="2" t="s">
+      <c r="G64" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="G64" s="4" t="s">
+      <c r="H64" t="s">
         <v>347</v>
-      </c>
-      <c r="H64" t="s">
-        <v>348</v>
       </c>
       <c r="I64">
         <v>3</v>
@@ -3918,25 +3979,25 @@
         <v>62</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C65" t="s">
         <v>349</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F65" s="2" t="s">
+      <c r="G65" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="G65" s="4" t="s">
+      <c r="H65" t="s">
         <v>352</v>
-      </c>
-      <c r="H65" t="s">
-        <v>353</v>
       </c>
       <c r="I65">
         <v>1</v>
@@ -3947,25 +4008,25 @@
         <v>63</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C66" t="s">
         <v>354</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F66" s="2" t="s">
+      <c r="G66" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="G66" s="4" t="s">
+      <c r="H66" t="s">
         <v>357</v>
-      </c>
-      <c r="H66" t="s">
-        <v>358</v>
       </c>
       <c r="I66">
         <v>2</v>
@@ -3976,25 +4037,25 @@
         <v>64</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C67" t="s">
         <v>359</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F67" s="2" t="s">
+      <c r="G67" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="H67" t="s">
         <v>362</v>
-      </c>
-      <c r="H67" t="s">
-        <v>363</v>
       </c>
       <c r="I67">
         <v>1</v>
@@ -4005,25 +4066,25 @@
         <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C68" t="s">
         <v>364</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="F68" s="2" t="s">
+      <c r="G68" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="G68" s="4" t="s">
+      <c r="H68" t="s">
         <v>367</v>
-      </c>
-      <c r="H68" t="s">
-        <v>368</v>
       </c>
       <c r="I68">
         <v>6</v>
@@ -4034,56 +4095,56 @@
         <v>66</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C69" t="s">
         <v>369</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="E69" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="E69" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F69" s="2" t="s">
+      <c r="G69" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="H69" t="s">
         <v>373</v>
-      </c>
-      <c r="H69" t="s">
-        <v>374</v>
       </c>
       <c r="I69">
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="10" customFormat="1" ht="54" x14ac:dyDescent="0.15">
-      <c r="A70" s="8">
+    <row r="70" spans="1:9" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+      <c r="A70" s="1">
         <v>67</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="C70" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D70" s="9" t="s">
+      <c r="D70" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="E70" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="F70" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="G70" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="F70" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="G70" s="11" t="s">
-        <v>488</v>
-      </c>
-      <c r="H70" s="10" t="s">
-        <v>485</v>
-      </c>
-      <c r="I70" s="10">
+      <c r="H70" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="I70" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4092,25 +4153,25 @@
         <v>68</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C71" t="s">
         <v>377</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E71" s="4" t="s">
+      <c r="F71" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="G71" s="4" t="s">
+      <c r="H71" t="s">
         <v>381</v>
-      </c>
-      <c r="H71" t="s">
-        <v>382</v>
       </c>
       <c r="I71">
         <v>1</v>
@@ -4121,25 +4182,25 @@
         <v>69</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C72" t="s">
+        <v>377</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="C72" t="s">
-        <v>378</v>
-      </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="F72" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="G72" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="G72" s="4" t="s">
+      <c r="H72" t="s">
         <v>387</v>
-      </c>
-      <c r="H72" t="s">
-        <v>388</v>
       </c>
       <c r="I72">
         <v>4</v>
@@ -4150,25 +4211,25 @@
         <v>70</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C73" t="s">
         <v>389</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="E73" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="F73" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="G73" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="G73" s="4" t="s">
+      <c r="H73" s="6" t="s">
         <v>394</v>
-      </c>
-      <c r="H73" s="6" t="s">
-        <v>395</v>
       </c>
       <c r="I73">
         <v>1</v>
@@ -4178,258 +4239,258 @@
       <c r="A74" s="1">
         <v>71</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="C74" t="s">
+        <v>395</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C74" t="s">
+      <c r="E74" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="G74" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>401</v>
-      </c>
       <c r="H74" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="8" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A75" s="1">
         <v>72</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="C75" t="s">
-        <v>403</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>406</v>
+      <c r="B75" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="H75" t="s">
-        <v>408</v>
-      </c>
-      <c r="I75">
+        <v>500</v>
+      </c>
+      <c r="H75" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="I75" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="135" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A76" s="1">
         <v>73</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="C76" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="H76" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="I76">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="108" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:9" ht="135" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
         <v>74</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C77" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="F77" s="2" t="s">
+      <c r="G77" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="H77" t="s">
         <v>413</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="H77" t="s">
-        <v>415</v>
       </c>
       <c r="I77">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:9" ht="108" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
         <v>75</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C78" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="H78" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="I78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="135" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A79" s="1">
         <v>76</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="C79" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>427</v>
+        <v>402</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="H79" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="I79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:9" ht="135" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
         <v>77</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C80" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="H80" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="I80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="135" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
         <v>78</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="C81" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="H81" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="I81">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="54" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:9" ht="135" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
         <v>79</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="C82" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="H82" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="I82">
         <v>1</v>
@@ -4440,25 +4501,25 @@
         <v>80</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="C83" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="H83" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="I83">
         <v>1</v>
@@ -4469,25 +4530,25 @@
         <v>81</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="C84" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="H84" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="I84">
         <v>1</v>
@@ -4498,25 +4559,25 @@
         <v>82</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="C85" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="H85" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="I85">
         <v>1</v>
@@ -4527,27 +4588,85 @@
         <v>83</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C86" t="s">
+        <v>464</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="H86" t="s">
+        <v>464</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="54" x14ac:dyDescent="0.15">
+      <c r="A87" s="1">
+        <v>84</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C87" t="s">
+        <v>470</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="C86" t="s">
+      <c r="E87" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="G87" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="H87" t="s">
         <v>475</v>
       </c>
-      <c r="G86" s="4" t="s">
-        <v>476</v>
-      </c>
-      <c r="H86" t="s">
-        <v>477</v>
-      </c>
-      <c r="I86">
+      <c r="I87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="8" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A88" s="1">
+        <v>85</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="H88" s="10">
+        <v>705430001</v>
+      </c>
+      <c r="I88" s="8">
         <v>1</v>
       </c>
     </row>
@@ -4622,18 +4741,18 @@
     <hyperlink ref="G72" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
     <hyperlink ref="G73" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
     <hyperlink ref="G74" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="G75" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="G76" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="G77" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="G78" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="G79" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="G80" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="G81" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="G82" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="G83" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="G84" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="G85" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="G86" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="G76" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="G77" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="G78" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="G79" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="G80" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="G81" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="G82" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="G83" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="G84" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="G85" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="G86" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="G87" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
     <hyperlink ref="E4" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
     <hyperlink ref="E5" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
     <hyperlink ref="E6" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
@@ -4699,22 +4818,26 @@
     <hyperlink ref="E72" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
     <hyperlink ref="E73" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
     <hyperlink ref="E74" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="E75" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="E76" r:id="rId144" display="https://www.ti.com/lit/ds/symlink/amc1301.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697614208280&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fgeneral%252Fdocs%252Fsuppproductinfo.tsp%253FdistId%253D10%2526gotoUrl%253Dhttps%253A%252F%252Fwww.ti.com%252Flit%252Fgpn%252Famc1301" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="E77" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="E78" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="E79" r:id="rId147" display="https://www.ti.com/lit/ds/symlink/opa2197.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1698207032697&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fgeneral%252Fdocs%252Fsuppproductinfo.tsp%253FdistId%253D10%2526gotoUrl%253Dhttps%253A%252F%252Fwww.ti.com%252Flit%252Fgpn%252Fopa2197" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="E80" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="E81" r:id="rId149" display="https://www.ti.com/lit/ds/symlink/tps54160a.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697682462443&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fgeneral%252Fdocs%252Fsuppproductinfo.tsp%253FdistId%253D10%2526gotoUrl%253Dhttps%253A%252F%252Fwww.ti.com%252Flit%252Fgpn%252Ftps54160a" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="E82" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="E83" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="E84" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="E85" r:id="rId153" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="E86" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="E76" r:id="rId143" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="E77" r:id="rId144" display="https://www.ti.com/lit/ds/symlink/amc1301.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697614208280&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fgeneral%252Fdocs%252Fsuppproductinfo.tsp%253FdistId%253D10%2526gotoUrl%253Dhttps%253A%252F%252Fwww.ti.com%252Flit%252Fgpn%252Famc1301" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="E78" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="E79" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="E80" r:id="rId147" display="https://www.ti.com/lit/ds/symlink/opa2197.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1698207032697&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fgeneral%252Fdocs%252Fsuppproductinfo.tsp%253FdistId%253D10%2526gotoUrl%253Dhttps%253A%252F%252Fwww.ti.com%252Flit%252Fgpn%252Fopa2197" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="E81" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="E82" r:id="rId149" display="https://www.ti.com/lit/ds/symlink/tps54160a.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1697682462443&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fgeneral%252Fdocs%252Fsuppproductinfo.tsp%253FdistId%253D10%2526gotoUrl%253Dhttps%253A%252F%252Fwww.ti.com%252Flit%252Fgpn%252Ftps54160a" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="E83" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="E84" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="E85" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="E86" r:id="rId153" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="E87" r:id="rId154" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
     <hyperlink ref="E50" r:id="rId155" xr:uid="{3B5A37A6-71DE-45B9-BAAD-06FE836F80EA}"/>
     <hyperlink ref="E70" r:id="rId156" xr:uid="{78A901DC-65A5-4C95-93CB-C934E3255132}"/>
+    <hyperlink ref="E88" r:id="rId157" xr:uid="{11324D34-126C-4518-B3FD-E62B9B8D6886}"/>
+    <hyperlink ref="G88" r:id="rId158" xr:uid="{A7C62A46-C021-479B-BA10-1A9259C7CE70}"/>
+    <hyperlink ref="E75" r:id="rId159" xr:uid="{8582B17A-B48B-4B14-9F45-AB67F3E9E204}"/>
+    <hyperlink ref="G75" r:id="rId160" xr:uid="{CC9D6EE0-BB07-4449-9F84-FBC5B26F17CE}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId157"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId161"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Substitute components in the bom that are out of stock.
</commit_message>
<xml_diff>
--- a/LTC6811_ESP32_BOM.xlsx
+++ b/LTC6811_ESP32_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\teTra\BMS\LTC6811_ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E69A77-6D95-4BDB-A140-3D3DAC9AEB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B990032-D450-4EEB-95BD-D99B227B4F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTC6811_ESP32" sheetId="1" r:id="rId1"/>
@@ -1528,22 +1528,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>1 µF ±10% 25V Ceramic Capacitor X7R 0603 (1608 Metric)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/4562/0603B105K250XD.pdf</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.digikey.jp/en/products/detail/nextgen-components/0603B105K250XD/14670931</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>0603B105K250XD</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>0.1 µF ±10% 50V Ceramic Capacitor X7R 0603 (1608 Metric)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1557,6 +1541,21 @@
   </si>
   <si>
     <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/609/CL10B104KB8NNNC_Spec.pdf</t>
+  </si>
+  <si>
+    <t>CL10A105KA8NNNC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.digikey.jp/en/products/detail/samsung-electro-mechanics/CL10A105KA8NNNC/3886760</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 µF ±10% 25V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/609/CL10A105KA8NNNC_Spec.pdf</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1643,24 +1642,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1680,7 +1667,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1720,47 +1707,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2253,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2671,90 +2655,90 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A16" s="1">
+    <row r="16" spans="1:9" s="15" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A16" s="13">
         <v>13</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>495</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>497</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="I16" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="15" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A17" s="13">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F17" s="17" t="s">
+        <v>501</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>500</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>499</v>
       </c>
-      <c r="G16" s="21" t="s">
-        <v>501</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>500</v>
-      </c>
-      <c r="I16" s="23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
-        <v>14</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="I17" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="20" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+      <c r="A18" s="13">
+        <v>15</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>496</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>495</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>497</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>498</v>
-      </c>
-      <c r="I17" s="23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.15">
-      <c r="A18" s="26">
-        <v>15</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>486</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="21" t="s">
         <v>491</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="19" t="s">
         <v>490</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="16" t="s">
         <v>492</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="20">
         <v>2</v>
       </c>
     </row>
@@ -4346,32 +4330,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="13" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A75" s="14">
+    <row r="75" spans="1:9" s="24" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A75" s="22">
         <v>72</v>
       </c>
-      <c r="B75" s="15" t="s">
+      <c r="B75" s="23" t="s">
         <v>483</v>
       </c>
-      <c r="C75" s="16" t="s">
+      <c r="C75" s="24" t="s">
         <v>488</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D75" s="23" t="s">
         <v>484</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E75" s="25" t="s">
         <v>489</v>
       </c>
-      <c r="F75" s="15" t="s">
+      <c r="F75" s="23" t="s">
         <v>485</v>
       </c>
-      <c r="G75" s="21" t="s">
+      <c r="G75" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="H75" s="16" t="s">
+      <c r="H75" s="24" t="s">
         <v>487</v>
       </c>
-      <c r="I75" s="16">
+      <c r="I75" s="24">
         <v>1</v>
       </c>
     </row>
@@ -4912,9 +4896,9 @@
     <hyperlink ref="G88" r:id="rId152" xr:uid="{A7C62A46-C021-479B-BA10-1A9259C7CE70}"/>
     <hyperlink ref="G18" r:id="rId153" xr:uid="{1BD06935-1FC1-4BB9-B495-A39E25F72230}"/>
     <hyperlink ref="G75" r:id="rId154" xr:uid="{9C191D6B-C100-4178-B2E7-02ACABBE1ECC}"/>
-    <hyperlink ref="E17" r:id="rId155" xr:uid="{00DFB778-4037-4FEC-923B-E1EC75B8D10C}"/>
-    <hyperlink ref="G17" r:id="rId156" xr:uid="{570B30A1-3ABE-4984-A8B3-1E9A8380BEF8}"/>
-    <hyperlink ref="G16" r:id="rId157" xr:uid="{994020A4-69E4-4CCC-B4EB-168EFD1CC578}"/>
+    <hyperlink ref="G16" r:id="rId155" xr:uid="{994020A4-69E4-4CCC-B4EB-168EFD1CC578}"/>
+    <hyperlink ref="G17" r:id="rId156" xr:uid="{AAE8FE46-07D4-47C7-AC8D-3D1B61BC31AC}"/>
+    <hyperlink ref="E17" r:id="rId157" xr:uid="{A039C161-577A-4EC6-BE9F-72F6946C412C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId158"/>

</xml_diff>